<commit_message>
Perbaiki contoh format impor, tambahkan sheet program dan peserta, expor semua data,
</commit_message>
<xml_diff>
--- a/assets/import/format_impor_peserta_bantuan.xlsx
+++ b/assets/import/format_impor_peserta_bantuan.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\manurung\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC54D9C-0D1E-49E2-8437-B27E3AD3BC0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41268124-235A-4C6C-909E-E9369CECDF6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="945" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Program" sheetId="2" r:id="rId1"/>
+    <sheet name="Peserta" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>No. Peserta</t>
   </si>
@@ -58,9 +59,6 @@
     <t>1. Sesuaikan kolom peserta (A) berdasarkan sasaran : - penduduk = nik, - keluarga = no. kk, - rumah tangga = no. rtm, - kelompok = kode</t>
   </si>
   <si>
-    <t>2. Kolom Peserta (A) dan kolom NIK (C) wajib di isi, yang lain jika kosong data diambil dari data penduduk berdasarkan kolom NIK ©</t>
-  </si>
-  <si>
     <t>5201142005716996</t>
   </si>
   <si>
@@ -83,20 +81,90 @@
   </si>
   <si>
     <t>RT 004 RW - Dusun Mangsit</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Nama Program</t>
+  </si>
+  <si>
+    <t>Bantuan Sosial Tunai</t>
+  </si>
+  <si>
+    <t>Sasaran Program</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Bantuan Kementerian Sosial Republik Indonesia</t>
+  </si>
+  <si>
+    <t>Asal Dana</t>
+  </si>
+  <si>
+    <t>Pusat</t>
+  </si>
+  <si>
+    <t>Rentang Waktu (Awal)</t>
+  </si>
+  <si>
+    <t>2020-04-01</t>
+  </si>
+  <si>
+    <t>Rentang Waktu (Akhir)</t>
+  </si>
+  <si>
+    <t>2020-12-31</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>2. Kolom Peserta (A) dan kolom NIK (C) wajib di isi, yang lain jika kosong data diambil dari data penduduk berdasarkan kolom NIK (C)</t>
+  </si>
+  <si>
+    <t>1. Sasaran : 1 = Penduduk, 2 = Keluarga, 3 = Rumah Tangga, 4 = Kelompok</t>
+  </si>
+  <si>
+    <t>2. Asal Dana : 1 = Pusat, 2 = Provinsi, 3 = Kab/Kota, 4 = Dana Desa, 5 = Lain-lain(Hibah)</t>
+  </si>
+  <si>
+    <t>3. Status : 1 = Aktif, 2 = Tidak Aktif (Status diatur otomatis sesuai rentang waktu)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,8 +177,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -133,17 +207,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,11 +561,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8C082F-6BC1-49A6-8236-34CCE45B6AA0}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="2" max="2" width="47.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -475,120 +695,121 @@
     <col min="7" max="7" width="31.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="A7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>